<commit_message>
Got frustrated but back now. Working in the server as will so will be harder to VC but we move... Going to try and use the sever for models and pull the output back out.
</commit_message>
<xml_diff>
--- a/Sandeel Data.xlsx
+++ b/Sandeel Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60d52dd049abb4b4/Pictures/Documents/MSc_Seal_SIA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{B2636446-E5E0-42E5-A412-A3E88A989AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F11E622C-0B08-4F7C-8CA3-FE0CE98E5E35}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{B2636446-E5E0-42E5-A412-A3E88A989AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40B01E72-DED9-4A97-9F8D-45196637A4F6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3E5F5977-9C99-4546-B4A0-510B1158BE21}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="24">
   <si>
     <t>Hyperoplus immaculatus</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Ammodytes marinus</t>
   </si>
   <si>
-    <t>St. Kilda</t>
-  </si>
-  <si>
     <t>d15N (or mean)</t>
   </si>
   <si>
@@ -92,13 +89,25 @@
     <t>Ammodytes tobianus</t>
   </si>
   <si>
-    <t>2005-2006</t>
-  </si>
-  <si>
     <t>North Sea</t>
   </si>
   <si>
     <t>Das et al., 2003 https://www.int-res.com/articles/meps2003/263/m263p287.pdf</t>
+  </si>
+  <si>
+    <t>2001-2002</t>
+  </si>
+  <si>
+    <t>Hyperoplus lanceolatus</t>
+  </si>
+  <si>
+    <t>2001-2001</t>
+  </si>
+  <si>
+    <t>Foula</t>
+  </si>
+  <si>
+    <t>Bearhop et al., 1999 https://www.jstor.org/stable/2655696?casa_token=LG2WgTk6tNcAAAAA%3AiksV4fDbxPgsqLOjlGVdUJJ0P7bQT2GQLaNpNMnLGNnCJwTF3AXbc5Txl_jvD7BSSC0uNJN28d9C6WHIQkFUHMP11eYahJprlNIsXvtzwes6bS61Ig&amp;seq=4</t>
   </si>
 </sst>
 </file>
@@ -152,6 +161,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -451,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{033E907F-477B-4F76-9E33-E549BD4890E7}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,19 +490,19 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -938,7 +951,7 @@
         <v>1995</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D17">
         <v>14</v>
@@ -956,7 +969,7 @@
         <v>0.6</v>
       </c>
       <c r="I17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -967,7 +980,7 @@
         <v>2005</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18">
         <v>6</v>
@@ -985,7 +998,7 @@
         <v>0.5</v>
       </c>
       <c r="I18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -996,7 +1009,7 @@
         <v>2005</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19">
         <v>6</v>
@@ -1014,18 +1027,18 @@
         <v>0.5</v>
       </c>
       <c r="I19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
         <v>17</v>
-      </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" t="s">
-        <v>19</v>
       </c>
       <c r="D20">
         <v>6</v>
@@ -1043,7 +1056,65 @@
         <v>0.2</v>
       </c>
       <c r="I20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21">
+        <v>7</v>
+      </c>
+      <c r="E21">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="F21">
+        <v>1.3</v>
+      </c>
+      <c r="G21">
+        <v>-16.399999999999999</v>
+      </c>
+      <c r="H21">
+        <v>0.4</v>
+      </c>
+      <c r="I21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>1996</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22">
+        <v>12</v>
+      </c>
+      <c r="E22">
+        <v>7.9</v>
+      </c>
+      <c r="F22">
+        <v>0.95</v>
+      </c>
+      <c r="G22">
+        <v>-17.5</v>
+      </c>
+      <c r="H22">
+        <v>0.75</v>
+      </c>
+      <c r="I22" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Everything except the posts
</commit_message>
<xml_diff>
--- a/Sandeel Data.xlsx
+++ b/Sandeel Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60d52dd049abb4b4/Pictures/Documents/MSc_Seal_SIA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{B2636446-E5E0-42E5-A412-A3E88A989AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40B01E72-DED9-4A97-9F8D-45196637A4F6}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{B2636446-E5E0-42E5-A412-A3E88A989AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BEDCA1B-E5DA-47BE-A820-01282816269D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3E5F5977-9C99-4546-B4A0-510B1158BE21}"/>
   </bookViews>
@@ -95,9 +95,6 @@
     <t>Das et al., 2003 https://www.int-res.com/articles/meps2003/263/m263p287.pdf</t>
   </si>
   <si>
-    <t>2001-2002</t>
-  </si>
-  <si>
     <t>Hyperoplus lanceolatus</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>Bearhop et al., 1999 https://www.jstor.org/stable/2655696?casa_token=LG2WgTk6tNcAAAAA%3AiksV4fDbxPgsqLOjlGVdUJJ0P7bQT2GQLaNpNMnLGNnCJwTF3AXbc5Txl_jvD7BSSC0uNJN28d9C6WHIQkFUHMP11eYahJprlNIsXvtzwes6bS61Ig&amp;seq=4</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G21" sqref="G20:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -951,7 +951,7 @@
         <v>1995</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17">
         <v>14</v>
@@ -1035,7 +1035,7 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
@@ -1061,10 +1061,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
         <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -1096,7 +1096,7 @@
         <v>1996</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22">
         <v>12</v>
@@ -1114,7 +1114,7 @@
         <v>0.75</v>
       </c>
       <c r="I22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>